<commit_message>
Atualizado por script em 20-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/italy_serie-c-group-b_2023-2024.xlsx
+++ b/2023/italy_serie-c-group-b_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V136"/>
+  <dimension ref="A1:V137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8945,22 +8945,22 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Spal</t>
+          <t>Ancona</t>
         </is>
       </c>
       <c r="G93" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Sestri Levante</t>
+          <t>Arezzo</t>
         </is>
       </c>
       <c r="I93" t="n">
         <v>0</v>
       </c>
       <c r="J93" t="n">
-        <v>1.76</v>
+        <v>2.16</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>
@@ -8968,15 +8968,15 @@
         </is>
       </c>
       <c r="L93" t="n">
-        <v>1.85</v>
+        <v>1.94</v>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>26/10/2023 18:29</t>
+          <t>26/10/2023 18:22</t>
         </is>
       </c>
       <c r="N93" t="n">
-        <v>3.21</v>
+        <v>2.9</v>
       </c>
       <c r="O93" t="inlineStr">
         <is>
@@ -8984,15 +8984,15 @@
         </is>
       </c>
       <c r="P93" t="n">
-        <v>3.03</v>
+        <v>3.4</v>
       </c>
       <c r="Q93" t="inlineStr">
         <is>
-          <t>26/10/2023 18:29</t>
+          <t>26/10/2023 18:22</t>
         </is>
       </c>
       <c r="R93" t="n">
-        <v>4.72</v>
+        <v>3.41</v>
       </c>
       <c r="S93" t="inlineStr">
         <is>
@@ -9000,16 +9000,16 @@
         </is>
       </c>
       <c r="T93" t="n">
-        <v>5.29</v>
+        <v>4</v>
       </c>
       <c r="U93" t="inlineStr">
         <is>
-          <t>26/10/2023 18:29</t>
+          <t>26/10/2023 18:22</t>
         </is>
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/spal-sestri-levante/WW8ctJKh/</t>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/ancona-arezzo/lp1QsBv0/</t>
         </is>
       </c>
     </row>
@@ -9037,22 +9037,22 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Ancona</t>
+          <t>Carrarese</t>
         </is>
       </c>
       <c r="G94" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>Arezzo</t>
+          <t>Pineto</t>
         </is>
       </c>
       <c r="I94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J94" t="n">
-        <v>2.16</v>
+        <v>1.67</v>
       </c>
       <c r="K94" t="inlineStr">
         <is>
@@ -9060,15 +9060,15 @@
         </is>
       </c>
       <c r="L94" t="n">
-        <v>1.94</v>
+        <v>1.52</v>
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>26/10/2023 18:22</t>
+          <t>26/10/2023 18:21</t>
         </is>
       </c>
       <c r="N94" t="n">
-        <v>2.9</v>
+        <v>3.29</v>
       </c>
       <c r="O94" t="inlineStr">
         <is>
@@ -9076,15 +9076,15 @@
         </is>
       </c>
       <c r="P94" t="n">
-        <v>3.4</v>
+        <v>3.84</v>
       </c>
       <c r="Q94" t="inlineStr">
         <is>
-          <t>26/10/2023 18:22</t>
+          <t>26/10/2023 18:21</t>
         </is>
       </c>
       <c r="R94" t="n">
-        <v>3.41</v>
+        <v>5.03</v>
       </c>
       <c r="S94" t="inlineStr">
         <is>
@@ -9092,16 +9092,16 @@
         </is>
       </c>
       <c r="T94" t="n">
-        <v>4</v>
+        <v>7.15</v>
       </c>
       <c r="U94" t="inlineStr">
         <is>
-          <t>26/10/2023 18:22</t>
+          <t>26/10/2023 18:21</t>
         </is>
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/ancona-arezzo/lp1QsBv0/</t>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/carrarese-pineto/W8jVtVg6/</t>
         </is>
       </c>
     </row>
@@ -9129,22 +9129,22 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Carrarese</t>
+          <t>Pontedera</t>
         </is>
       </c>
       <c r="G95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Pineto</t>
+          <t>Vis Pesaro</t>
         </is>
       </c>
       <c r="I95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J95" t="n">
-        <v>1.67</v>
+        <v>1.84</v>
       </c>
       <c r="K95" t="inlineStr">
         <is>
@@ -9152,15 +9152,15 @@
         </is>
       </c>
       <c r="L95" t="n">
-        <v>1.52</v>
+        <v>1.82</v>
       </c>
       <c r="M95" t="inlineStr">
         <is>
-          <t>26/10/2023 18:21</t>
+          <t>26/10/2023 18:02</t>
         </is>
       </c>
       <c r="N95" t="n">
-        <v>3.29</v>
+        <v>3.08</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -9168,15 +9168,15 @@
         </is>
       </c>
       <c r="P95" t="n">
-        <v>3.84</v>
+        <v>3.34</v>
       </c>
       <c r="Q95" t="inlineStr">
         <is>
-          <t>26/10/2023 18:21</t>
+          <t>26/10/2023 18:02</t>
         </is>
       </c>
       <c r="R95" t="n">
-        <v>5.03</v>
+        <v>4.28</v>
       </c>
       <c r="S95" t="inlineStr">
         <is>
@@ -9184,16 +9184,16 @@
         </is>
       </c>
       <c r="T95" t="n">
-        <v>7.15</v>
+        <v>4.8</v>
       </c>
       <c r="U95" t="inlineStr">
         <is>
-          <t>26/10/2023 18:21</t>
+          <t>26/10/2023 18:02</t>
         </is>
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/carrarese-pineto/W8jVtVg6/</t>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/us-pontedera-vis-pesaro/McJNnLsP/</t>
         </is>
       </c>
     </row>
@@ -9313,22 +9313,22 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Pontedera</t>
+          <t>Spal</t>
         </is>
       </c>
       <c r="G97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Vis Pesaro</t>
+          <t>Sestri Levante</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>0</v>
       </c>
       <c r="J97" t="n">
-        <v>1.84</v>
+        <v>1.76</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
@@ -9336,15 +9336,15 @@
         </is>
       </c>
       <c r="L97" t="n">
-        <v>1.82</v>
+        <v>1.85</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>26/10/2023 18:02</t>
+          <t>26/10/2023 18:29</t>
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.08</v>
+        <v>3.21</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -9352,15 +9352,15 @@
         </is>
       </c>
       <c r="P97" t="n">
-        <v>3.34</v>
+        <v>3.03</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
-          <t>26/10/2023 18:02</t>
+          <t>26/10/2023 18:29</t>
         </is>
       </c>
       <c r="R97" t="n">
-        <v>4.28</v>
+        <v>4.72</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
@@ -9368,16 +9368,16 @@
         </is>
       </c>
       <c r="T97" t="n">
-        <v>4.8</v>
+        <v>5.29</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
-          <t>26/10/2023 18:02</t>
+          <t>26/10/2023 18:29</t>
         </is>
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/us-pontedera-vis-pesaro/McJNnLsP/</t>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/spal-sestri-levante/WW8ctJKh/</t>
         </is>
       </c>
     </row>
@@ -9497,22 +9497,22 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Juventus U23</t>
+          <t>Torres</t>
         </is>
       </c>
       <c r="G99" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Olbia</t>
+          <t>Spal</t>
         </is>
       </c>
       <c r="I99" t="n">
         <v>1</v>
       </c>
       <c r="J99" t="n">
-        <v>2.08</v>
+        <v>1.79</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -9520,15 +9520,15 @@
         </is>
       </c>
       <c r="L99" t="n">
-        <v>2.06</v>
+        <v>2</v>
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>29/10/2023 13:33</t>
+          <t>29/10/2023 13:53</t>
         </is>
       </c>
       <c r="N99" t="n">
-        <v>2.94</v>
+        <v>3.12</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -9536,15 +9536,15 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>3.17</v>
+        <v>3.18</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
-          <t>29/10/2023 13:50</t>
+          <t>29/10/2023 13:53</t>
         </is>
       </c>
       <c r="R99" t="n">
-        <v>3.57</v>
+        <v>4.5</v>
       </c>
       <c r="S99" t="inlineStr">
         <is>
@@ -9552,16 +9552,16 @@
         </is>
       </c>
       <c r="T99" t="n">
-        <v>3.6</v>
+        <v>4.12</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
-          <t>29/10/2023 13:33</t>
+          <t>29/10/2023 13:54</t>
         </is>
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/juventus-olbia/Q7ezL8lp/</t>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/sassari-torres-spal/Q3uZuAQ9/</t>
         </is>
       </c>
     </row>
@@ -9589,22 +9589,22 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Torres</t>
+          <t>Juventus U23</t>
         </is>
       </c>
       <c r="G100" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>Spal</t>
+          <t>Olbia</t>
         </is>
       </c>
       <c r="I100" t="n">
         <v>1</v>
       </c>
       <c r="J100" t="n">
-        <v>1.79</v>
+        <v>2.08</v>
       </c>
       <c r="K100" t="inlineStr">
         <is>
@@ -9612,15 +9612,15 @@
         </is>
       </c>
       <c r="L100" t="n">
-        <v>2</v>
+        <v>2.06</v>
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>29/10/2023 13:53</t>
+          <t>29/10/2023 13:33</t>
         </is>
       </c>
       <c r="N100" t="n">
-        <v>3.12</v>
+        <v>2.94</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -9628,15 +9628,15 @@
         </is>
       </c>
       <c r="P100" t="n">
-        <v>3.18</v>
+        <v>3.17</v>
       </c>
       <c r="Q100" t="inlineStr">
         <is>
-          <t>29/10/2023 13:53</t>
+          <t>29/10/2023 13:50</t>
         </is>
       </c>
       <c r="R100" t="n">
-        <v>4.5</v>
+        <v>3.57</v>
       </c>
       <c r="S100" t="inlineStr">
         <is>
@@ -9644,16 +9644,16 @@
         </is>
       </c>
       <c r="T100" t="n">
-        <v>4.12</v>
+        <v>3.6</v>
       </c>
       <c r="U100" t="inlineStr">
         <is>
-          <t>29/10/2023 13:54</t>
+          <t>29/10/2023 13:33</t>
         </is>
       </c>
       <c r="V100" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/sassari-torres-spal/Q3uZuAQ9/</t>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/juventus-olbia/Q7ezL8lp/</t>
         </is>
       </c>
     </row>
@@ -9957,22 +9957,22 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Vis Pesaro</t>
+          <t>Perugia</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Pineto</t>
+          <t>Entella</t>
         </is>
       </c>
       <c r="I104" t="n">
         <v>1</v>
       </c>
       <c r="J104" t="n">
-        <v>2.21</v>
+        <v>2.12</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
@@ -9980,7 +9980,7 @@
         </is>
       </c>
       <c r="L104" t="n">
-        <v>2.65</v>
+        <v>1.92</v>
       </c>
       <c r="M104" t="inlineStr">
         <is>
@@ -9988,7 +9988,7 @@
         </is>
       </c>
       <c r="N104" t="n">
-        <v>2.88</v>
+        <v>3.01</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
@@ -9996,7 +9996,7 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>2.76</v>
+        <v>3.28</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
@@ -10004,7 +10004,7 @@
         </is>
       </c>
       <c r="R104" t="n">
-        <v>3.31</v>
+        <v>3.36</v>
       </c>
       <c r="S104" t="inlineStr">
         <is>
@@ -10012,7 +10012,7 @@
         </is>
       </c>
       <c r="T104" t="n">
-        <v>3.16</v>
+        <v>4.34</v>
       </c>
       <c r="U104" t="inlineStr">
         <is>
@@ -10021,7 +10021,7 @@
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/vis-pesaro-pineto/KQvwuUuG/</t>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/perugia-entella/hEmMrCti/</t>
         </is>
       </c>
     </row>
@@ -10049,7 +10049,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Perugia</t>
+          <t>Cesena</t>
         </is>
       </c>
       <c r="G105" t="n">
@@ -10057,63 +10057,63 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Entella</t>
+          <t>Carrarese</t>
         </is>
       </c>
       <c r="I105" t="n">
         <v>1</v>
       </c>
       <c r="J105" t="n">
-        <v>2.12</v>
+        <v>1.84</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>26/10/2023 22:12</t>
+          <t>26/10/2023 21:12</t>
         </is>
       </c>
       <c r="L105" t="n">
-        <v>1.92</v>
+        <v>1.65</v>
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>30/10/2023 20:36</t>
+          <t>30/10/2023 20:42</t>
         </is>
       </c>
       <c r="N105" t="n">
-        <v>3.01</v>
+        <v>3.08</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
-          <t>26/10/2023 22:12</t>
+          <t>26/10/2023 21:12</t>
         </is>
       </c>
       <c r="P105" t="n">
-        <v>3.28</v>
+        <v>3.44</v>
       </c>
       <c r="Q105" t="inlineStr">
         <is>
-          <t>30/10/2023 20:36</t>
+          <t>30/10/2023 20:42</t>
         </is>
       </c>
       <c r="R105" t="n">
-        <v>3.36</v>
+        <v>4.28</v>
       </c>
       <c r="S105" t="inlineStr">
         <is>
-          <t>26/10/2023 22:12</t>
+          <t>26/10/2023 21:12</t>
         </is>
       </c>
       <c r="T105" t="n">
-        <v>4.34</v>
+        <v>6.35</v>
       </c>
       <c r="U105" t="inlineStr">
         <is>
-          <t>30/10/2023 20:36</t>
+          <t>30/10/2023 20:42</t>
         </is>
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/perugia-entella/hEmMrCti/</t>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/cesena-carrarese/W6w2wH4B/</t>
         </is>
       </c>
     </row>
@@ -10141,30 +10141,30 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Cesena</t>
+          <t>Arezzo</t>
         </is>
       </c>
       <c r="G106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>Carrarese</t>
+          <t>Gubbio</t>
         </is>
       </c>
       <c r="I106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J106" t="n">
-        <v>1.84</v>
+        <v>2.34</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>26/10/2023 21:12</t>
+          <t>26/10/2023 22:12</t>
         </is>
       </c>
       <c r="L106" t="n">
-        <v>1.65</v>
+        <v>3.4</v>
       </c>
       <c r="M106" t="inlineStr">
         <is>
@@ -10172,15 +10172,15 @@
         </is>
       </c>
       <c r="N106" t="n">
-        <v>3.08</v>
+        <v>2.85</v>
       </c>
       <c r="O106" t="inlineStr">
         <is>
-          <t>26/10/2023 21:12</t>
+          <t>26/10/2023 22:12</t>
         </is>
       </c>
       <c r="P106" t="n">
-        <v>3.44</v>
+        <v>2.96</v>
       </c>
       <c r="Q106" t="inlineStr">
         <is>
@@ -10188,15 +10188,15 @@
         </is>
       </c>
       <c r="R106" t="n">
-        <v>4.28</v>
+        <v>3.09</v>
       </c>
       <c r="S106" t="inlineStr">
         <is>
-          <t>26/10/2023 21:12</t>
+          <t>26/10/2023 22:12</t>
         </is>
       </c>
       <c r="T106" t="n">
-        <v>6.35</v>
+        <v>2.35</v>
       </c>
       <c r="U106" t="inlineStr">
         <is>
@@ -10205,7 +10205,7 @@
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/cesena-carrarese/W6w2wH4B/</t>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/arezzo-gubbio/xpvbvck5/</t>
         </is>
       </c>
     </row>
@@ -10233,7 +10233,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Arezzo</t>
+          <t>Vis Pesaro</t>
         </is>
       </c>
       <c r="G107" t="n">
@@ -10241,14 +10241,14 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>Gubbio</t>
+          <t>Pineto</t>
         </is>
       </c>
       <c r="I107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J107" t="n">
-        <v>2.34</v>
+        <v>2.21</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -10256,15 +10256,15 @@
         </is>
       </c>
       <c r="L107" t="n">
-        <v>3.4</v>
+        <v>2.65</v>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>30/10/2023 20:42</t>
+          <t>30/10/2023 20:36</t>
         </is>
       </c>
       <c r="N107" t="n">
-        <v>2.85</v>
+        <v>2.88</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -10272,15 +10272,15 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>2.96</v>
+        <v>2.76</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>30/10/2023 20:42</t>
+          <t>30/10/2023 20:36</t>
         </is>
       </c>
       <c r="R107" t="n">
-        <v>3.09</v>
+        <v>3.31</v>
       </c>
       <c r="S107" t="inlineStr">
         <is>
@@ -10288,16 +10288,16 @@
         </is>
       </c>
       <c r="T107" t="n">
-        <v>2.35</v>
+        <v>3.16</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>30/10/2023 20:42</t>
+          <t>30/10/2023 20:36</t>
         </is>
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/arezzo-gubbio/xpvbvck5/</t>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/vis-pesaro-pineto/KQvwuUuG/</t>
         </is>
       </c>
     </row>
@@ -12809,71 +12809,71 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Carrarese</t>
+          <t>Gubbio</t>
         </is>
       </c>
       <c r="G135" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>Spal</t>
+          <t>Sestri Levante</t>
         </is>
       </c>
       <c r="I135" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J135" t="n">
-        <v>1.89</v>
+        <v>1.53</v>
       </c>
       <c r="K135" t="inlineStr">
         <is>
-          <t>16/11/2023 09:12</t>
+          <t>16/11/2023 18:12</t>
         </is>
       </c>
       <c r="L135" t="n">
-        <v>1.66</v>
+        <v>1.6</v>
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>19/11/2023 16:12</t>
+          <t>19/11/2023 16:11</t>
         </is>
       </c>
       <c r="N135" t="n">
-        <v>3.15</v>
+        <v>3.75</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
-          <t>16/11/2023 09:12</t>
+          <t>16/11/2023 18:12</t>
         </is>
       </c>
       <c r="P135" t="n">
-        <v>3.43</v>
+        <v>3.61</v>
       </c>
       <c r="Q135" t="inlineStr">
         <is>
-          <t>19/11/2023 16:12</t>
+          <t>19/11/2023 16:11</t>
         </is>
       </c>
       <c r="R135" t="n">
-        <v>3.89</v>
+        <v>5.85</v>
       </c>
       <c r="S135" t="inlineStr">
         <is>
-          <t>16/11/2023 09:12</t>
+          <t>16/11/2023 18:12</t>
         </is>
       </c>
       <c r="T135" t="n">
-        <v>6.12</v>
+        <v>6.56</v>
       </c>
       <c r="U135" t="inlineStr">
         <is>
-          <t>19/11/2023 16:12</t>
+          <t>19/11/2023 16:11</t>
         </is>
       </c>
       <c r="V135" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/carrarese-spal/SE8YbOWl/</t>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/gubbio-sestri-levante/EVApdMG7/</t>
         </is>
       </c>
     </row>
@@ -12901,71 +12901,163 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Gubbio</t>
+          <t>Carrarese</t>
         </is>
       </c>
       <c r="G136" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Sestri Levante</t>
+          <t>Spal</t>
         </is>
       </c>
       <c r="I136" t="n">
+        <v>0</v>
+      </c>
+      <c r="J136" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>16/11/2023 09:12</t>
+        </is>
+      </c>
+      <c r="L136" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>19/11/2023 16:12</t>
+        </is>
+      </c>
+      <c r="N136" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>16/11/2023 09:12</t>
+        </is>
+      </c>
+      <c r="P136" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>19/11/2023 16:12</t>
+        </is>
+      </c>
+      <c r="R136" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>16/11/2023 09:12</t>
+        </is>
+      </c>
+      <c r="T136" t="n">
+        <v>6.12</v>
+      </c>
+      <c r="U136" t="inlineStr">
+        <is>
+          <t>19/11/2023 16:12</t>
+        </is>
+      </c>
+      <c r="V136" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/carrarese-spal/SE8YbOWl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>italy</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>serie-c-group-b</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E137" s="2" t="n">
+        <v>45250.77083333334</v>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Vis Pesaro</t>
+        </is>
+      </c>
+      <c r="G137" t="n">
+        <v>1</v>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>Torres</t>
+        </is>
+      </c>
+      <c r="I137" t="n">
         <v>2</v>
       </c>
-      <c r="J136" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="K136" t="inlineStr">
-        <is>
-          <t>16/11/2023 18:12</t>
-        </is>
-      </c>
-      <c r="L136" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="M136" t="inlineStr">
-        <is>
-          <t>19/11/2023 16:11</t>
-        </is>
-      </c>
-      <c r="N136" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="O136" t="inlineStr">
-        <is>
-          <t>16/11/2023 18:12</t>
-        </is>
-      </c>
-      <c r="P136" t="n">
-        <v>3.61</v>
-      </c>
-      <c r="Q136" t="inlineStr">
-        <is>
-          <t>19/11/2023 16:11</t>
-        </is>
-      </c>
-      <c r="R136" t="n">
-        <v>5.85</v>
-      </c>
-      <c r="S136" t="inlineStr">
-        <is>
-          <t>16/11/2023 18:12</t>
-        </is>
-      </c>
-      <c r="T136" t="n">
-        <v>6.56</v>
-      </c>
-      <c r="U136" t="inlineStr">
-        <is>
-          <t>19/11/2023 16:11</t>
-        </is>
-      </c>
-      <c r="V136" t="inlineStr">
-        <is>
-          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/gubbio-sestri-levante/EVApdMG7/</t>
+      <c r="J137" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>16/11/2023 09:12</t>
+        </is>
+      </c>
+      <c r="L137" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>20/11/2023 18:25</t>
+        </is>
+      </c>
+      <c r="N137" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="O137" t="inlineStr">
+        <is>
+          <t>16/11/2023 09:12</t>
+        </is>
+      </c>
+      <c r="P137" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="Q137" t="inlineStr">
+        <is>
+          <t>20/11/2023 18:25</t>
+        </is>
+      </c>
+      <c r="R137" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="S137" t="inlineStr">
+        <is>
+          <t>16/11/2023 09:12</t>
+        </is>
+      </c>
+      <c r="T137" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="U137" t="inlineStr">
+        <is>
+          <t>20/11/2023 18:25</t>
+        </is>
+      </c>
+      <c r="V137" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/italy/serie-c-group-b/vis-pesaro-sassari-torres/6Le0DNor/</t>
         </is>
       </c>
     </row>

</xml_diff>